<commit_message>
[HuyLQ] - FE - Update UI
</commit_message>
<xml_diff>
--- a/FjapFE/src/vn.fpt.edu.pages/staffAcademic/importSchedule/Assets/ScheduleImportTemplate.xlsx
+++ b/FjapFE/src/vn.fpt.edu.pages/staffAcademic/importSchedule/Assets/ScheduleImportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FJAP\FjapFE\src\vn.fpt.edu.pages\staffAcademic\importSchedule\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E86FE7-D730-47AD-83B7-36FD92CCD89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3056DBF5-87A8-4F1B-B14B-5B845F632C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{E55EA64E-A8F1-4908-BF04-CC8CB4C243AC}"/>
   </bookViews>
@@ -38,91 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Slot</t>
-  </si>
-  <si>
-    <t>room</t>
-  </si>
-  <si>
-    <t>DayOfWeek</t>
-  </si>
-  <si>
-    <t>Class Name</t>
-  </si>
-  <si>
-    <t>Lecture</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Class Name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is the Name of Class, example:  SP26-N5-JPN101-01
--</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Input the</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> lecturer’s email ID (characters before @ only)
--</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> DayOfWeek</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is represented by numbers 2–8, corresponding to Monday–Sunday.</t>
-    </r>
-  </si>
-  <si>
     <t>SP26-N5-JPN101-01</t>
   </si>
   <si>
@@ -134,12 +49,156 @@
   <si>
     <t>No.</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Class Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is the Name of Class, example:  SP26-N5-JPN101-01
+-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Input the</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lecturer’s email ID (characters before @ only)
+-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DayOfWeek</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is represented by numbers 2–8, corresponding to Monday–Sunday.
+- You can use Slot: 2,3 - DayOfWeek 2,3 will to  create 2 rows 
+                          row 1: slot 2 - DayOfWeek 2
+                          row 2: slot 3 - DayOfWeek 3
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Slot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lecture </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Class Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> *</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DayOfWeek</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Room</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +219,18 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -182,7 +253,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -190,17 +261,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96322039-A1BA-454F-9BF5-71B450386A9F}">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,218 +638,386 @@
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4">
+        <v>102</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>102</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-    </row>
-    <row r="17" spans="10:17" x14ac:dyDescent="0.3">
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="10:17" x14ac:dyDescent="0.3">
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>